<commit_message>
including countries runs fully (if not correctly)
</commit_message>
<xml_diff>
--- a/tests/data/countries_data.xlsx
+++ b/tests/data/countries_data.xlsx
@@ -1,29 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Theano\PycharmProjects\DIMPACT\eam-core\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEF509F-7ED0-4211-9763-34AED1EB74FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9A2DA7-825E-431E-84E5-97DB38F06422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="348" windowWidth="12264" windowHeight="8616" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="carbon_intensity" sheetId="4" r:id="rId2"/>
     <sheet name="changes" sheetId="2" r:id="rId3"/>
     <sheet name="metadata" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>variable</t>
   </si>
@@ -82,6 +92,30 @@
     <t>id</t>
   </si>
   <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>carbon_intensity</t>
+  </si>
+  <si>
+    <t>kg/kWh</t>
+  </si>
+  <si>
+    <t>31.7.18</t>
+  </si>
+  <si>
+    <t>DS change all to lowercase</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
     <t>power_latop</t>
   </si>
   <si>
@@ -118,9 +152,6 @@
     <t>energy_intensity_network</t>
   </si>
   <si>
-    <t>exp</t>
-  </si>
-  <si>
     <t>kWh/GB</t>
   </si>
   <si>
@@ -130,34 +161,7 @@
     <t>bps</t>
   </si>
   <si>
-    <t>carbon_intensity</t>
-  </si>
-  <si>
-    <t>kg/kWh</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>31.7.18</t>
-  </si>
-  <si>
-    <t>DS change all to lowercase</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>DE</t>
+    <t>region</t>
   </si>
 </sst>
 </file>
@@ -552,7 +556,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,16 +622,16 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -642,16 +646,16 @@
         <v>43617</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -659,16 +663,16 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -683,10 +687,10 @@
         <v>43617</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -694,10 +698,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -715,7 +719,7 @@
         <v>42522</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="S4">
         <v>2</v>
@@ -723,10 +727,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3">
         <v>40000000</v>
@@ -744,7 +748,7 @@
         <v>43617</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="S5">
         <v>3</v>
@@ -752,10 +756,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>0.5</v>
@@ -773,43 +777,14 @@
         <v>43617</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="S6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7">
-        <v>0.5</v>
-      </c>
-      <c r="F7">
-        <v>-0.2</v>
-      </c>
-      <c r="G7">
-        <v>0.1</v>
-      </c>
-      <c r="H7">
-        <v>0.05</v>
-      </c>
-      <c r="I7" s="2">
-        <v>43617</v>
-      </c>
-      <c r="J7" t="s">
-        <v>36</v>
-      </c>
-      <c r="S7">
-        <v>5</v>
-      </c>
+      <c r="I7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E9" s="3"/>
@@ -821,10 +796,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA40DB2E-E0E2-4F9F-B6A5-FFA36E109B26}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,54 +808,60 @@
     <col min="4" max="4" width="30.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="C2">
         <v>0.5</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
       </c>
       <c r="D2">
         <v>0.1</v>
       </c>
       <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3">
         <v>0.4</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>0.1</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.05</v>
       </c>
     </row>
@@ -903,10 +884,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +908,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
fixed bug where interpolation crashed
</commit_message>
<xml_diff>
--- a/tests/data/countries_data.xlsx
+++ b/tests/data/countries_data.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="carbon_intensity" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="time_laptop" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="changes" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="metadata" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
@@ -82,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -90,6 +90,7 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -399,10 +400,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -507,29 +508,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>power_latop</t>
+          <t>carbon_intensity</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>interp</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>linear</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
-        </is>
+          <t>exp</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="H2" t="n">
         <v>0.05</v>
@@ -539,26 +533,11 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="P2" s="3" t="inlineStr">
-        <is>
-          <t>what does it mean? How do collect this info?</t>
-        </is>
-      </c>
-      <c r="Q2" s="3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="R2" s="3" t="inlineStr">
-        <is>
-          <t>power draw of laptop</t>
+          <t>kg/kWh</t>
         </is>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -681,22 +660,29 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>carbon_intensity</t>
+          <t>power_latop</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>exp</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.5</v>
+          <t>interp</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
+        </is>
       </c>
       <c r="F6" t="n">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="H6" t="n">
         <v>0.05</v>
@@ -706,16 +692,30 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>kg/kWh</t>
-        </is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="P6" s="3" t="inlineStr">
+        <is>
+          <t>what does it mean? How do collect this info?</t>
+        </is>
+      </c>
+      <c r="Q6" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R6" s="3" t="inlineStr">
+        <is>
+          <t>power draw of laptop</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="I7" s="2" t="n"/>
-    </row>
-    <row r="8"/>
-    <row r="9">
-      <c r="E9" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -730,15 +730,11 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="11.77734375"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="30.77734375"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -778,47 +774,51 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>0.5</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":100, "2031-06-01":95}</t>
+        </is>
       </c>
       <c r="D2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>0.05</v>
       </c>
-      <c r="G2" t="n">
-        <v>4</v>
+      <c r="G2" s="7" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>DE</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>0.4</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":100, "2031-06-01":95}</t>
+        </is>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
         <v>0.05</v>
       </c>
       <c r="G3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -836,7 +836,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
trying to fix hdf5
</commit_message>
<xml_diff>
--- a/tests/data/countries_data.xlsx
+++ b/tests/data/countries_data.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="time_laptop" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="energy_intensity_network" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="changes" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="metadata" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
@@ -82,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -90,7 +90,6 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -402,8 +401,8 @@
   </sheetPr>
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:S6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -508,22 +507,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>carbon_intensity</t>
+          <t>power_latop</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>exp</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0.5</v>
+          <t>interp</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
+        </is>
       </c>
       <c r="F2" t="n">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="H2" t="n">
         <v>0.05</v>
@@ -533,11 +539,26 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>kg/kWh</t>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="P2" s="3" t="inlineStr">
+        <is>
+          <t>what does it mean? How do collect this info?</t>
+        </is>
+      </c>
+      <c r="Q2" s="3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R2" s="3" t="inlineStr">
+        <is>
+          <t>power draw of laptop</t>
         </is>
       </c>
       <c r="S2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -660,29 +681,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>power_latop</t>
+          <t>carbon_intensity</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>interp</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>linear</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>{"2020-01-01":10, "2031-06-01":9.5}</t>
-        </is>
+          <t>exp</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="H6" t="n">
         <v>0.05</v>
@@ -692,26 +706,11 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="P6" s="3" t="inlineStr">
-        <is>
-          <t>what does it mean? How do collect this info?</t>
-        </is>
-      </c>
-      <c r="Q6" s="3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="R6" s="3" t="inlineStr">
-        <is>
-          <t>power draw of laptop</t>
+          <t>kg/kWh</t>
         </is>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -730,8 +729,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -779,21 +778,19 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{"2020-01-01":100, "2031-06-01":95}</t>
-        </is>
+      <c r="C2" t="n">
+        <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G2" s="7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="n">
         <v>6</v>
       </c>
     </row>
@@ -803,19 +800,17 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{"2020-01-01":100, "2031-06-01":95}</t>
-        </is>
+      <c r="C3" t="n">
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="E3" t="n">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G3" t="n">
         <v>7</v>
@@ -823,7 +818,6 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>